<commit_message>
update database and landing page
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/parvathykrishnank/Documents/GitHub/CCS RTD/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7737801D-A924-6145-9078-7E467881AA44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="58">
   <si>
     <t>ID</t>
   </si>
@@ -67,95 +61,140 @@
     <t>Link</t>
   </si>
   <si>
-    <t>ETT-MT</t>
+    <t>Short Description</t>
+  </si>
+  <si>
+    <t>Disruption</t>
+  </si>
+  <si>
+    <t>Asset Types</t>
+  </si>
+  <si>
+    <t>WB</t>
+  </si>
+  <si>
+    <t>HCT-1</t>
+  </si>
+  <si>
+    <t>HCT-2</t>
+  </si>
+  <si>
+    <t>WTW</t>
+  </si>
+  <si>
+    <t>WB12</t>
+  </si>
+  <si>
+    <t>CP-ETT-fsJ o_x000D_4P</t>
   </si>
   <si>
     <t>Maximum Temperature</t>
   </si>
   <si>
+    <t>Maximum Precipitation</t>
+  </si>
+  <si>
+    <t>Heat Wave</t>
+  </si>
+  <si>
+    <t>Cumulative Precipitation</t>
+  </si>
+  <si>
     <t>Exposure Tolerance Threshold</t>
   </si>
   <si>
+    <t>Hazard Criticality Threshold</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
     <t>degree celsius</t>
   </si>
   <si>
+    <t>mm/day</t>
+  </si>
+  <si>
+    <t>120</t>
+  </si>
+  <si>
+    <t>140</t>
+  </si>
+  <si>
+    <t>160</t>
+  </si>
+  <si>
+    <t>\</t>
+  </si>
+  <si>
+    <t>180</t>
+  </si>
+  <si>
     <t>number of days</t>
   </si>
   <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>Number of days</t>
+  </si>
+  <si>
     <t>Heat</t>
   </si>
   <si>
+    <t>Precipitation</t>
+  </si>
+  <si>
     <t>A1.2, A1.3, A1.6</t>
   </si>
   <si>
+    <t>A1.2,A1.3,A1.6</t>
+  </si>
+  <si>
+    <t>A1.3,A1.6</t>
+  </si>
+  <si>
     <t>Armenia, Georgia, Vietnam</t>
   </si>
   <si>
+    <t>Global</t>
+  </si>
+  <si>
+    <t>Vietnam</t>
+  </si>
+  <si>
     <t>Test Description</t>
   </si>
   <si>
+    <t>Test</t>
+  </si>
+  <si>
     <t>https://github.com/Analytics-for-a-Better-World/GPBP_Analytics_Tools</t>
   </si>
   <si>
-    <t>HCT-1</t>
-  </si>
-  <si>
-    <t>Hazard Criticality Threshold</t>
-  </si>
-  <si>
-    <t>Global</t>
-  </si>
-  <si>
-    <t>HCT-2</t>
-  </si>
-  <si>
-    <t>Maximum Precipitation</t>
-  </si>
-  <si>
-    <t>mm</t>
-  </si>
-  <si>
-    <t>Precipitation</t>
-  </si>
-  <si>
-    <t>HW-HCT-Og!S O_B</t>
-  </si>
-  <si>
-    <t>Heat Wave</t>
-  </si>
-  <si>
-    <t>A1.2,A1.3,A1.6</t>
-  </si>
-  <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>MT-ETT-aU9u	$v*</t>
-  </si>
-  <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t>120</t>
-  </si>
-  <si>
-    <t>170</t>
-  </si>
-  <si>
-    <t>190</t>
-  </si>
-  <si>
-    <t>Number of days</t>
-  </si>
-  <si>
-    <t>\</t>
+    <t>http://gpbprtd.eu.pythonanywhere.com/</t>
+  </si>
+  <si>
+    <t>Moderate</t>
+  </si>
+  <si>
+    <t>Severe</t>
+  </si>
+  <si>
+    <t>Urban Roads</t>
+  </si>
+  <si>
+    <t>Highways</t>
+  </si>
+  <si>
+    <t>Public Buildings</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -166,7 +205,17 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -201,28 +250,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -510,25 +557,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:R21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="2" width="23.33203125" customWidth="1"/>
-    <col min="3" max="3" width="23.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="56.5" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -574,22 +610,31 @@
       <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="D2">
         <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="F2">
         <v>120</v>
@@ -601,33 +646,42 @@
         <v>190</v>
       </c>
       <c r="J2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K2" t="s">
+        <v>41</v>
+      </c>
+      <c r="L2" t="s">
+        <v>43</v>
+      </c>
+      <c r="M2" t="s">
+        <v>46</v>
+      </c>
+      <c r="N2" t="s">
+        <v>49</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="P2" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>53</v>
+      </c>
+      <c r="R2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
+      <c r="A3" t="s">
         <v>19</v>
       </c>
-      <c r="K2" t="s">
-        <v>20</v>
-      </c>
-      <c r="L2" t="s">
-        <v>21</v>
-      </c>
-      <c r="M2" t="s">
-        <v>22</v>
-      </c>
-      <c r="N2" t="s">
-        <v>23</v>
-      </c>
-      <c r="O2" t="s">
+      <c r="B3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F3">
         <v>30</v>
@@ -642,33 +696,42 @@
         <v>45</v>
       </c>
       <c r="J3" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="K3" t="s">
+        <v>41</v>
+      </c>
+      <c r="L3" t="s">
+        <v>43</v>
+      </c>
+      <c r="M3" t="s">
+        <v>47</v>
+      </c>
+      <c r="N3" t="s">
+        <v>49</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="P3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>54</v>
+      </c>
+      <c r="R3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
+      <c r="A4" t="s">
         <v>20</v>
       </c>
-      <c r="L3" t="s">
-        <v>21</v>
-      </c>
-      <c r="M3" t="s">
-        <v>27</v>
-      </c>
-      <c r="N3" t="s">
-        <v>23</v>
-      </c>
-      <c r="O3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>28</v>
-      </c>
       <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
         <v>29</v>
-      </c>
-      <c r="C4" t="s">
-        <v>26</v>
       </c>
       <c r="F4">
         <v>30</v>
@@ -683,33 +746,42 @@
         <v>70</v>
       </c>
       <c r="J4" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K4" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="L4" t="s">
+        <v>43</v>
+      </c>
+      <c r="M4" t="s">
+        <v>47</v>
+      </c>
+      <c r="N4" t="s">
+        <v>49</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="P4" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>54</v>
+      </c>
+      <c r="R4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="A5" t="s">
         <v>21</v>
       </c>
-      <c r="M4" t="s">
-        <v>27</v>
-      </c>
-      <c r="N4" t="s">
-        <v>23</v>
-      </c>
-      <c r="O4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>32</v>
-      </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F5">
         <v>30</v>
@@ -724,68 +796,148 @@
         <v>45</v>
       </c>
       <c r="J5" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="K5" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="L5" t="s">
+        <v>44</v>
+      </c>
+      <c r="M5" t="s">
+        <v>47</v>
+      </c>
+      <c r="N5" t="s">
+        <v>50</v>
+      </c>
+      <c r="P5" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>53</v>
+      </c>
+      <c r="R5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6">
+        <v>40</v>
+      </c>
+      <c r="E6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6">
+        <v>120</v>
+      </c>
+      <c r="G6">
+        <v>170</v>
+      </c>
+      <c r="H6">
+        <v>190</v>
+      </c>
+      <c r="J6" t="s">
+        <v>40</v>
+      </c>
+      <c r="K6" t="s">
+        <v>41</v>
+      </c>
+      <c r="L6" t="s">
+        <v>44</v>
+      </c>
+      <c r="M6" t="s">
+        <v>47</v>
+      </c>
+      <c r="N6" t="s">
+        <v>50</v>
+      </c>
+      <c r="P6" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>54</v>
+      </c>
+      <c r="R6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18">
+      <c r="I20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" t="s">
+        <v>30</v>
+      </c>
+      <c r="E21" t="s">
+        <v>32</v>
+      </c>
+      <c r="F21" t="s">
+        <v>33</v>
+      </c>
+      <c r="G21" t="s">
         <v>34</v>
       </c>
-      <c r="M5" t="s">
-        <v>27</v>
-      </c>
-      <c r="N5" t="s">
+      <c r="H21" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="I21" t="s">
         <v>37</v>
       </c>
-      <c r="E6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" t="s">
-        <v>38</v>
-      </c>
-      <c r="G6" t="s">
-        <v>39</v>
-      </c>
-      <c r="H6" t="s">
-        <v>40</v>
-      </c>
-      <c r="J6" t="s">
-        <v>41</v>
-      </c>
-      <c r="K6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L6" t="s">
-        <v>34</v>
-      </c>
-      <c r="M6" t="s">
-        <v>27</v>
-      </c>
-      <c r="N6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I20" t="s">
+      <c r="J21" t="s">
+        <v>32</v>
+      </c>
+      <c r="K21" t="s">
         <v>42</v>
+      </c>
+      <c r="L21" t="s">
+        <v>45</v>
+      </c>
+      <c r="M21" t="s">
+        <v>48</v>
+      </c>
+      <c r="N21" t="s">
+        <v>50</v>
+      </c>
+      <c r="O21" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="P21" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>54</v>
+      </c>
+      <c r="R21" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <hyperlinks>
+    <hyperlink ref="O2" r:id="rId1"/>
+    <hyperlink ref="O3" r:id="rId2"/>
+    <hyperlink ref="O4" r:id="rId3"/>
+    <hyperlink ref="O21" r:id="rId4"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>